<commit_message>
Added many new case studies and files
</commit_message>
<xml_diff>
--- a/bin/pkgSeleniumCoursePart9/CaseStudyPart9/test-data/TestCaseTestsAndStatus.xlsx
+++ b/bin/pkgSeleniumCoursePart9/CaseStudyPart9/test-data/TestCaseTestsAndStatus.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgri\eclipse-workspace-jee-2019-03\Ed_GSeleniumProject\src\pkgSeleniumCoursePart9\CaseStudyPart9\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA894571-6D17-43FD-8844-837D3B1A3674}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCE65EA-03C1-450A-9A0C-AC8105D52847}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15158" yWindow="-13575" windowWidth="21601" windowHeight="11513" xr2:uid="{8A909AE7-29B9-4C15-A5B5-345E4B7D58FB}"/>
+    <workbookView xWindow="-17872" yWindow="-16275" windowWidth="20880" windowHeight="13875" xr2:uid="{8A909AE7-29B9-4C15-A5B5-345E4B7D58FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,38 +30,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Times Run</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
   </si>
   <si>
-    <t>2019-07-21 at 20:42:10 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 20:42:25 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 20:42:41 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 20:56:38 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 20:57:27 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 20:57:34 CDT</t>
-  </si>
-  <si>
     <t>2019-07-21 at 21:00:39 CDT</t>
   </si>
   <si>
@@ -107,15 +86,6 @@
     <t>2019-07-21 at 21:21:37 CDT</t>
   </si>
   <si>
-    <t>2019-07-21 at 21:21:40 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:21:45 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:22:26 CDT</t>
-  </si>
-  <si>
     <t>2019-07-21 at 21:22:29 CDT</t>
   </si>
   <si>
@@ -128,41 +98,43 @@
     <t>2019-07-21 at 21:23:18 CDT</t>
   </si>
   <si>
-    <t>2019-07-21 at 21:23:58 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:24:01 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:24:07 CDT</t>
-  </si>
-  <si>
     <t>Note: Actul failure. Edureka popped a advertisement during test run.</t>
   </si>
   <si>
-    <t>2019-07-21 at 21:31:39 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:31:42 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:31:46 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:33:22 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:33:26 CDT</t>
-  </si>
-  <si>
-    <t>2019-07-21 at 21:33:30 CDT</t>
+    <t>2019-07-21 at 21:34:23 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:34:27 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:34:31 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:35:00 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:35:03 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:35:08 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:38:12 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:38:15 CDT</t>
+  </si>
+  <si>
+    <t>2019-07-21 at 21:38:19 CDT</t>
+  </si>
+  <si>
+    <t>Times when Last Test in Test Run Completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -290,33 +262,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,21 +578,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3620D7-7EAA-4288-B83F-DA435254D9DA}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="14.0" collapsed="true"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" style="3" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -655,47 +600,53 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>2</v>
@@ -703,64 +654,67 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -768,10 +722,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -779,10 +730,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -790,7 +738,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -798,7 +746,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -808,16 +756,16 @@
       <c r="B19" s="21" t="s">
         <v>2</v>
       </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,7 +773,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -833,7 +781,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -841,7 +789,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -849,7 +797,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -857,7 +805,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,7 +813,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -873,7 +821,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -881,82 +829,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s" s="34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s" s="35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s" s="37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s" s="38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" t="s" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>